<commit_message>
Final files for the Hackathon
</commit_message>
<xml_diff>
--- a/Back end/Recieve_mail/Email_data.xlsx
+++ b/Back end/Recieve_mail/Email_data.xlsx
@@ -1,34 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="324" yWindow="564" windowWidth="6396" windowHeight="5244"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>116_Deepak Kumar &lt;deepakkumar737373@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Introduction to Algorithms,Operating System,Natraj Pencils,Apsara non-dust</t>
+  </si>
+  <si>
+    <t>"Medium Daily Digest" &lt;noreply@medium.com&gt;</t>
+  </si>
+  <si>
+    <t>Today's highlights</t>
+  </si>
+  <si>
+    <t>Neha Jhawar &lt;nehajhawar1609@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Natraj Pencils</t>
+  </si>
+  <si>
+    <t>TechGig Webinar &lt;expertspeak@techgig.com&gt;</t>
+  </si>
+  <si>
+    <t>Mailtrack Notification &lt;notification@mailtrack.io&gt;</t>
+  </si>
+  <si>
+    <t>non dust eraser</t>
+  </si>
+  <si>
+    <t>kundan Prakash Jha &lt;kundan.ext123@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Operating system</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,15 +86,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,68 +388,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.77734375" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>EMAIL</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>PRODUCT</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>116_Deepak Kumar &lt;deepakkumar737373@gmail.com&gt;</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Introduction to Algorithms,Operating System,Natraj Pencils,Apsara non-dust</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>"Medium Daily Digest" &lt;noreply@medium.com&gt;</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Today's highlights</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Neha Jhawar &lt;nehajhawar1609@gmail.com&gt;</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Natraj Pencils</t>
-        </is>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>